<commit_message>
Market data. 2021-2024 added
</commit_message>
<xml_diff>
--- a/data/IEEE9/Market Data/ieee9_market_data_2020.xlsx
+++ b/data/IEEE9/Market Data/ieee9_market_data_2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\IEEE9\Market Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE592686-EA6A-4399-99F7-EF9523E17D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3EB418-F15F-44AD-9BD2-62ED04FFD62A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8445" yWindow="7170" windowWidth="21600" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5070" yWindow="4815" windowWidth="21600" windowHeight="12660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -1324,7 +1324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1847,8 +1847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59BA0F2A-A97B-42BF-BD16-0283FFE6BEE7}">
   <dimension ref="A1:Y6"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:Y4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>